<commit_message>
return dataframe and update model
</commit_message>
<xml_diff>
--- a/data/data_couches_original.xlsx
+++ b/data/data_couches_original.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20730"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\JUSAU\Desktop\LANG_SCRIPT\LangageScript\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Stone\Desktop\lang_script\LangageScript\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E02CF0C2-6D69-4EB8-B7DB-A8607F8E6ACA}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3DB2BD42-EE4D-462E-A8F7-E0C0A70FE787}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="6000" yWindow="1815" windowWidth="15375" windowHeight="7875" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -63,9 +63,6 @@
     <t>g- Lupilu</t>
   </si>
   <si>
-    <t xml:space="preserve">e- Pamp. Activ.   </t>
-  </si>
-  <si>
     <t>f- Carref.Baby</t>
   </si>
   <si>
@@ -106,6 +103,9 @@
   </si>
   <si>
     <t>Max_value</t>
+  </si>
+  <si>
+    <t>e- Pamp. Activ.</t>
   </si>
 </sst>
 </file>
@@ -468,7 +468,7 @@
   <dimension ref="A1:H13"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="F7" sqref="F7"/>
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75"/>
@@ -484,28 +484,28 @@
   <sheetData>
     <row r="1" spans="1:8">
       <c r="A1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="C1" t="s">
+        <v>16</v>
+      </c>
+      <c r="D1" t="s">
         <v>19</v>
       </c>
-      <c r="C1" t="s">
-        <v>17</v>
-      </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>20</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>21</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>22</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>23</v>
-      </c>
-      <c r="H1" t="s">
-        <v>24</v>
       </c>
     </row>
     <row r="2" spans="1:8">
@@ -597,7 +597,7 @@
         <v>12.5</v>
       </c>
       <c r="F5" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="G5">
         <v>7</v>
@@ -608,7 +608,7 @@
     </row>
     <row r="6" spans="1:8">
       <c r="A6" s="1" t="s">
-        <v>10</v>
+        <v>24</v>
       </c>
       <c r="B6" t="s">
         <v>8</v>
@@ -620,7 +620,7 @@
         <v>12.5</v>
       </c>
       <c r="F6" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="G6">
         <v>0</v>
@@ -631,7 +631,7 @@
     </row>
     <row r="7" spans="1:8">
       <c r="A7" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B7" s="2" t="s">
         <v>7</v>
@@ -651,7 +651,7 @@
         <v>7</v>
       </c>
       <c r="C8" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D8" s="3">
         <v>12</v>
@@ -659,13 +659,13 @@
     </row>
     <row r="9" spans="1:8">
       <c r="A9" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B9" t="s">
         <v>8</v>
       </c>
       <c r="C9" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D9" s="3">
         <v>12</v>
@@ -673,13 +673,13 @@
     </row>
     <row r="10" spans="1:8">
       <c r="A10" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C10" t="s">
         <v>13</v>
-      </c>
-      <c r="B10" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="C10" t="s">
-        <v>14</v>
       </c>
       <c r="D10" s="3">
         <v>9.5</v>
@@ -687,13 +687,13 @@
     </row>
     <row r="11" spans="1:8">
       <c r="A11" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B11" s="2" t="s">
         <v>7</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D11" s="3">
         <v>9.5</v>
@@ -707,7 +707,7 @@
         <v>7</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D12" s="3">
         <v>9.5</v>
@@ -721,7 +721,7 @@
         <v>8</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D13" s="3">
         <v>6.5</v>

</xml_diff>